<commit_message>
Correct bug in indst/SYSoIEbV
</commit_message>
<xml_diff>
--- a/InputData/indst/SYSoIEbV/Start Year Shr of Indst Eqpt by Vintage.xlsx
+++ b/InputData/indst/SYSoIEbV/Start Year Shr of Indst Eqpt by Vintage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\indst\SYSoIEbV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAE7569-DD82-49E4-A7EF-762651A416F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65045131-C304-48E8-9E4E-51A861F124A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10284" yWindow="528" windowWidth="27900" windowHeight="18012" xr2:uid="{F6F8D70B-4981-4594-95C7-E07791D5C609}"/>
+    <workbookView xWindow="6000" yWindow="312" windowWidth="27900" windowHeight="18012" xr2:uid="{F6F8D70B-4981-4594-95C7-E07791D5C609}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -61,15 +61,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="249">
   <si>
     <t>Source:</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Snapshot of Age Distribution of Existing Equipment (Row must sum to 1)</t>
   </si>
   <si>
     <t>US EPA</t>
@@ -805,13 +799,31 @@
     <t>SYSoIEbV Start Year Share of Industrial Equipment by Vintage</t>
   </si>
   <si>
-    <t>We then convert to a snapshot of the age of each cohort of equipment at any given year</t>
-  </si>
-  <si>
-    <t>and then assign those years to vintages starting immediately prior to the first simulated</t>
-  </si>
-  <si>
-    <t>year and going backward by 50 years.</t>
+    <t>Percentage of Start Year Eqpt by Age</t>
+  </si>
+  <si>
+    <t>Finally, we convert each year's surviving fraction to a percentage of the total, assuming that</t>
+  </si>
+  <si>
+    <t>the system is in steady state (meaning the same quantity of new industrial equipment is</t>
+  </si>
+  <si>
+    <t>deployed each year).</t>
+  </si>
+  <si>
+    <t>The sum of the row in SYSoIEbV must sum to 1.</t>
+  </si>
+  <si>
+    <t>These parameters were chosen manually so as to align the</t>
+  </si>
+  <si>
+    <t>Equipment Age</t>
+  </si>
+  <si>
+    <t>Weibull curve as close as possible to years 1 - 29 of  the "Surviving</t>
+  </si>
+  <si>
+    <t>Share of Equipment (Raw)" curve.</t>
   </si>
 </sst>
 </file>
@@ -865,15 +877,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -905,11 +923,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -944,6 +1024,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,10 +1085,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1021,7 +1111,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Snapshot of Age Distribution of Existing Equipment (Row must sum to 1)</c:v>
+                  <c:v>Percentage of Start Year Eqpt by Age</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1045,154 +1135,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>2.6150091858251345E-3</c:v>
+                  <c:v>6.3880424710375722E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.1544757227045572E-3</c:v>
+                  <c:v>6.3358147578421301E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3774823353250532E-2</c:v>
+                  <c:v>6.2475898923969687E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9275669922149241E-2</c:v>
+                  <c:v>6.1241332540332052E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4523292727533286E-2</c:v>
+                  <c:v>5.9670666880471963E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9407198843811155E-2</c:v>
+                  <c:v>5.7787197238371522E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3834275964629623E-2</c:v>
+                  <c:v>5.5620182556684494E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.7728226791890251E-2</c:v>
+                  <c:v>5.3203768460591126E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.1030137629935015E-2</c:v>
+                  <c:v>5.0575873874383399E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.3699063554975437E-2</c:v>
+                  <c:v>4.7777040159170989E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.571223339725683E-2</c:v>
+                  <c:v>4.4849267121907947E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.7064725842333344E-2</c:v>
+                  <c:v>4.1834869769455905E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.7768581473379368E-2</c:v>
+                  <c:v>3.8775391934481963E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.7851380175605751E-2</c:v>
+                  <c:v>3.5710611015631277E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.7354354957917399E-2</c:v>
+                  <c:v>3.2677663523481532E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.6330140678369047E-2</c:v>
+                  <c:v>2.9710314815928063E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.4840272649322499E-2</c:v>
+                  <c:v>2.6838389042682251E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.2952557155367943E-2</c:v>
+                  <c:v>2.4087367502602947E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.0738434630281872E-2</c:v>
+                  <c:v>2.1478155884034345E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.827044775206212E-2</c:v>
+                  <c:v>1.9027013668366639E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.5619912364544648E-2</c:v>
+                  <c:v>1.6745632706200733E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.2854870440236994E-2</c:v>
+                  <c:v>1.464134690196635E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.0038382886396264E-2</c:v>
+                  <c:v>1.2717451240743808E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.7227197490210825E-2</c:v>
+                  <c:v>1.0973606130413696E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.4470805217893771E-2</c:v>
+                  <c:v>9.4063021858778219E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.1810877745534557E-2</c:v>
+                  <c:v>8.0093610382538979E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.9281061554515685E-2</c:v>
+                  <c:v>6.7744493318285534E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.6907089904774603E-2</c:v>
+                  <c:v>5.6915855493568854E-3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.4707163909978713E-2</c:v>
+                  <c:v>4.7496224302932752E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.2692547868771803E-2</c:v>
+                  <c:v>3.9366912592997665E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0868321764506451E-2</c:v>
+                  <c:v>3.2405979587188634E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9.2342350138447729E-3</c:v>
+                  <c:v>2.6491645002322903E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.7856095396596492E-3</c:v>
+                  <c:v>2.1505124765873172E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.5142463855848223E-3</c:v>
+                  <c:v>1.7332886065554501E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.4092976646944249E-3</c:v>
+                  <c:v>1.3868343934000575E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.4580739526365112E-3</c:v>
+                  <c:v>1.1013040715007754E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.6467656742491285E-3</c:v>
+                  <c:v>8.6773634967242809E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.9610650716444878E-3</c:v>
+                  <c:v>6.7808631872770661E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.3866825805346267E-3</c:v>
+                  <c:v>5.2522428621511478E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.9097576064443841E-3</c:v>
+                  <c:v>4.0290830179875493E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.5171686316344021E-3</c:v>
+                  <c:v>3.0573682093763767E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.1967512543959785E-3</c:v>
+                  <c:v>2.2908740360373135E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9.3743521238418524E-4</c:v>
+                  <c:v>1.6904663694182346E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.2931278684615916E-4</c:v>
+                  <c:v>1.223356767814851E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.6365138676737212E-4</c:v>
+                  <c:v>8.6234983160760257E-5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.3286275766671886E-4</c:v>
+                  <c:v>5.8511027962194154E-5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.3044034177507329E-4</c:v>
+                  <c:v>3.7347014498544394E-5</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.5087501887319789E-4</c:v>
+                  <c:v>2.1278993721771694E-5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.8955794509232236E-4</c:v>
+                  <c:v>9.1382034038435014E-6</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.4267761930706339E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1246,10 +1336,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1305,10 +1392,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1361,7 +1445,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -3607,154 +3695,154 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.4267761930706339E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.8955794509232236E-4</c:v>
+                  <c:v>9.1382034038435014E-6</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2.5087501887319789E-4</c:v>
+                  <c:v>2.1278993721771694E-5</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>3.3044034177507329E-4</c:v>
+                  <c:v>3.7347014498544394E-5</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.3286275766671886E-4</c:v>
+                  <c:v>5.8511027962194154E-5</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5.6365138676737212E-4</c:v>
+                  <c:v>8.6234983160760257E-5</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>7.2931278684615916E-4</c:v>
+                  <c:v>1.223356767814851E-4</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>9.3743521238418524E-4</c:v>
+                  <c:v>1.6904663694182346E-4</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.1967512543959785E-3</c:v>
+                  <c:v>2.2908740360373135E-4</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.5171686316344021E-3</c:v>
+                  <c:v>3.0573682093763767E-4</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.9097576064443841E-3</c:v>
+                  <c:v>4.0290830179875493E-4</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.3866825805346267E-3</c:v>
+                  <c:v>5.2522428621511478E-4</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2.9610650716444878E-3</c:v>
+                  <c:v>6.7808631872770661E-4</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>3.6467656742491285E-3</c:v>
+                  <c:v>8.6773634967242809E-4</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.4580739526365112E-3</c:v>
+                  <c:v>1.1013040715007754E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>5.4092976646944249E-3</c:v>
+                  <c:v>1.3868343934000575E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>6.5142463855848223E-3</c:v>
+                  <c:v>1.7332886065554501E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>7.7856095396596492E-3</c:v>
+                  <c:v>2.1505124765873172E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>9.2342350138447729E-3</c:v>
+                  <c:v>2.6491645002322903E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.0868321764506451E-2</c:v>
+                  <c:v>3.2405979587188634E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.2692547868771803E-2</c:v>
+                  <c:v>3.9366912592997665E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.4707163909978713E-2</c:v>
+                  <c:v>4.7496224302932752E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.6907089904774603E-2</c:v>
+                  <c:v>5.6915855493568854E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.9281061554515685E-2</c:v>
+                  <c:v>6.7744493318285534E-3</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>2.1810877745534557E-2</c:v>
+                  <c:v>8.0093610382538979E-3</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2.4470805217893771E-2</c:v>
+                  <c:v>9.4063021858778219E-3</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>2.7227197490210825E-2</c:v>
+                  <c:v>1.0973606130413696E-2</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>3.0038382886396264E-2</c:v>
+                  <c:v>1.2717451240743808E-2</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>3.2854870440236994E-2</c:v>
+                  <c:v>1.464134690196635E-2</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>3.5619912364544648E-2</c:v>
+                  <c:v>1.6745632706200733E-2</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>3.827044775206212E-2</c:v>
+                  <c:v>1.9027013668366639E-2</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>4.0738434630281872E-2</c:v>
+                  <c:v>2.1478155884034345E-2</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>4.2952557155367943E-2</c:v>
+                  <c:v>2.4087367502602947E-2</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>4.4840272649322499E-2</c:v>
+                  <c:v>2.6838389042682251E-2</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>4.6330140678369047E-2</c:v>
+                  <c:v>2.9710314815928063E-2</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>4.7354354957917399E-2</c:v>
+                  <c:v>3.2677663523481532E-2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>4.7851380175605751E-2</c:v>
+                  <c:v>3.5710611015631277E-2</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>4.7768581473379368E-2</c:v>
+                  <c:v>3.8775391934481963E-2</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>4.7064725842333344E-2</c:v>
+                  <c:v>4.1834869769455905E-2</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>4.571223339725683E-2</c:v>
+                  <c:v>4.4849267121907947E-2</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>4.3699063554975437E-2</c:v>
+                  <c:v>4.7777040159170989E-2</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>4.1030137629935015E-2</c:v>
+                  <c:v>5.0575873874383399E-2</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>3.7728226791890251E-2</c:v>
+                  <c:v>5.3203768460591126E-2</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>3.3834275964629623E-2</c:v>
+                  <c:v>5.5620182556684494E-2</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.9407198843811155E-2</c:v>
+                  <c:v>5.7787197238371522E-2</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2.4523292727533286E-2</c:v>
+                  <c:v>5.9670666880471963E-2</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>1.9275669922149241E-2</c:v>
+                  <c:v>6.1241332540332052E-2</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>1.3774823353250532E-2</c:v>
+                  <c:v>6.2475898923969687E-2</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>8.1544757227045572E-3</c:v>
+                  <c:v>6.3358147578421301E-2</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>2.6150091858251345E-3</c:v>
+                  <c:v>6.3880424710375722E-2</c:v>
                 </c:pt>
                 <c:pt idx="130">
                   <c:v>0</c:v>
@@ -6278,7 +6366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{277D797A-29C7-42A2-8124-270B3E72FA7C}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6289,7 +6377,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -6297,7 +6385,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -6307,78 +6395,84 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>27</v>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>28</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>242</v>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>243</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
         <v>244</v>
       </c>
+      <c r="B23" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6399,7 +6493,7 @@
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>246</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6557,7 +6651,7 @@
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <f t="array" ref="B2:AF2">TRANSPOSE('MOVES3 Table C-1'!D3:D33)</f>
@@ -6656,7 +6750,7 @@
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -6784,7 +6878,7 @@
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <f t="shared" ref="B4:AF4" si="1">1-_xlfn.WEIBULL.DIST(B1,$B$9,$B$11,TRUE)</f>
@@ -6993,7 +7087,7 @@
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <f t="shared" ref="B5" si="3">B4-(B1/$AZ$1)*$AZ$4</f>
@@ -7199,234 +7293,244 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>240</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <f>B5-C5</f>
-        <v>2.6150091858251345E-3</v>
+        <f>C5/SUM($C$5:$AZ$5)</f>
+        <v>6.3880424710375722E-2</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:AZ6" si="35">C5-D5</f>
-        <v>8.1544757227045572E-3</v>
+        <f t="shared" ref="D6:AZ6" si="35">D5/SUM($C$5:$AZ$5)</f>
+        <v>6.3358147578421301E-2</v>
       </c>
       <c r="E6">
         <f t="shared" si="35"/>
-        <v>1.3774823353250532E-2</v>
+        <v>6.2475898923969687E-2</v>
       </c>
       <c r="F6">
         <f t="shared" si="35"/>
-        <v>1.9275669922149241E-2</v>
+        <v>6.1241332540332052E-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="35"/>
-        <v>2.4523292727533286E-2</v>
+        <v>5.9670666880471963E-2</v>
       </c>
       <c r="H6">
         <f t="shared" si="35"/>
-        <v>2.9407198843811155E-2</v>
+        <v>5.7787197238371522E-2</v>
       </c>
       <c r="I6">
         <f t="shared" si="35"/>
-        <v>3.3834275964629623E-2</v>
+        <v>5.5620182556684494E-2</v>
       </c>
       <c r="J6">
         <f t="shared" si="35"/>
-        <v>3.7728226791890251E-2</v>
+        <v>5.3203768460591126E-2</v>
       </c>
       <c r="K6">
         <f t="shared" si="35"/>
-        <v>4.1030137629935015E-2</v>
+        <v>5.0575873874383399E-2</v>
       </c>
       <c r="L6">
         <f t="shared" si="35"/>
-        <v>4.3699063554975437E-2</v>
+        <v>4.7777040159170989E-2</v>
       </c>
       <c r="M6">
         <f t="shared" si="35"/>
-        <v>4.571223339725683E-2</v>
+        <v>4.4849267121907947E-2</v>
       </c>
       <c r="N6">
         <f t="shared" si="35"/>
-        <v>4.7064725842333344E-2</v>
+        <v>4.1834869769455905E-2</v>
       </c>
       <c r="O6">
         <f t="shared" si="35"/>
-        <v>4.7768581473379368E-2</v>
+        <v>3.8775391934481963E-2</v>
       </c>
       <c r="P6">
         <f t="shared" si="35"/>
-        <v>4.7851380175605751E-2</v>
+        <v>3.5710611015631277E-2</v>
       </c>
       <c r="Q6">
         <f t="shared" si="35"/>
-        <v>4.7354354957917399E-2</v>
+        <v>3.2677663523481532E-2</v>
       </c>
       <c r="R6">
         <f t="shared" si="35"/>
-        <v>4.6330140678369047E-2</v>
+        <v>2.9710314815928063E-2</v>
       </c>
       <c r="S6">
         <f t="shared" si="35"/>
-        <v>4.4840272649322499E-2</v>
+        <v>2.6838389042682251E-2</v>
       </c>
       <c r="T6">
         <f t="shared" si="35"/>
-        <v>4.2952557155367943E-2</v>
+        <v>2.4087367502602947E-2</v>
       </c>
       <c r="U6">
         <f t="shared" si="35"/>
-        <v>4.0738434630281872E-2</v>
+        <v>2.1478155884034345E-2</v>
       </c>
       <c r="V6">
         <f t="shared" si="35"/>
-        <v>3.827044775206212E-2</v>
+        <v>1.9027013668366639E-2</v>
       </c>
       <c r="W6">
         <f t="shared" si="35"/>
-        <v>3.5619912364544648E-2</v>
+        <v>1.6745632706200733E-2</v>
       </c>
       <c r="X6">
         <f t="shared" si="35"/>
-        <v>3.2854870440236994E-2</v>
+        <v>1.464134690196635E-2</v>
       </c>
       <c r="Y6">
         <f t="shared" si="35"/>
-        <v>3.0038382886396264E-2</v>
+        <v>1.2717451240743808E-2</v>
       </c>
       <c r="Z6">
         <f t="shared" si="35"/>
-        <v>2.7227197490210825E-2</v>
+        <v>1.0973606130413696E-2</v>
       </c>
       <c r="AA6">
         <f t="shared" si="35"/>
-        <v>2.4470805217893771E-2</v>
+        <v>9.4063021858778219E-3</v>
       </c>
       <c r="AB6">
         <f t="shared" si="35"/>
-        <v>2.1810877745534557E-2</v>
+        <v>8.0093610382538979E-3</v>
       </c>
       <c r="AC6">
         <f t="shared" si="35"/>
-        <v>1.9281061554515685E-2</v>
+        <v>6.7744493318285534E-3</v>
       </c>
       <c r="AD6">
         <f t="shared" si="35"/>
-        <v>1.6907089904774603E-2</v>
+        <v>5.6915855493568854E-3</v>
       </c>
       <c r="AE6">
         <f t="shared" si="35"/>
-        <v>1.4707163909978713E-2</v>
+        <v>4.7496224302932752E-3</v>
       </c>
       <c r="AF6">
         <f t="shared" si="35"/>
-        <v>1.2692547868771803E-2</v>
+        <v>3.9366912592997665E-3</v>
       </c>
       <c r="AG6">
         <f t="shared" si="35"/>
-        <v>1.0868321764506451E-2</v>
+        <v>3.2405979587188634E-3</v>
       </c>
       <c r="AH6">
         <f t="shared" si="35"/>
-        <v>9.2342350138447729E-3</v>
+        <v>2.6491645002322903E-3</v>
       </c>
       <c r="AI6">
         <f t="shared" si="35"/>
-        <v>7.7856095396596492E-3</v>
+        <v>2.1505124765873172E-3</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="35"/>
-        <v>6.5142463855848223E-3</v>
+        <v>1.7332886065554501E-3</v>
       </c>
       <c r="AK6">
         <f t="shared" si="35"/>
-        <v>5.4092976646944249E-3</v>
+        <v>1.3868343934000575E-3</v>
       </c>
       <c r="AL6">
         <f t="shared" si="35"/>
-        <v>4.4580739526365112E-3</v>
+        <v>1.1013040715007754E-3</v>
       </c>
       <c r="AM6">
         <f t="shared" si="35"/>
-        <v>3.6467656742491285E-3</v>
+        <v>8.6773634967242809E-4</v>
       </c>
       <c r="AN6">
         <f t="shared" si="35"/>
-        <v>2.9610650716444878E-3</v>
+        <v>6.7808631872770661E-4</v>
       </c>
       <c r="AO6">
         <f t="shared" si="35"/>
-        <v>2.3866825805346267E-3</v>
+        <v>5.2522428621511478E-4</v>
       </c>
       <c r="AP6">
         <f t="shared" si="35"/>
-        <v>1.9097576064443841E-3</v>
+        <v>4.0290830179875493E-4</v>
       </c>
       <c r="AQ6">
         <f t="shared" si="35"/>
-        <v>1.5171686316344021E-3</v>
+        <v>3.0573682093763767E-4</v>
       </c>
       <c r="AR6">
         <f t="shared" si="35"/>
-        <v>1.1967512543959785E-3</v>
+        <v>2.2908740360373135E-4</v>
       </c>
       <c r="AS6">
         <f t="shared" si="35"/>
-        <v>9.3743521238418524E-4</v>
+        <v>1.6904663694182346E-4</v>
       </c>
       <c r="AT6">
         <f t="shared" si="35"/>
-        <v>7.2931278684615916E-4</v>
+        <v>1.223356767814851E-4</v>
       </c>
       <c r="AU6">
         <f t="shared" si="35"/>
-        <v>5.6365138676737212E-4</v>
+        <v>8.6234983160760257E-5</v>
       </c>
       <c r="AV6">
         <f t="shared" si="35"/>
-        <v>4.3286275766671886E-4</v>
+        <v>5.8511027962194154E-5</v>
       </c>
       <c r="AW6">
         <f t="shared" si="35"/>
-        <v>3.3044034177507329E-4</v>
+        <v>3.7347014498544394E-5</v>
       </c>
       <c r="AX6">
         <f t="shared" si="35"/>
-        <v>2.5087501887319789E-4</v>
+        <v>2.1278993721771694E-5</v>
       </c>
       <c r="AY6">
         <f t="shared" si="35"/>
-        <v>1.8955794509232236E-4</v>
+        <v>9.1382034038435014E-6</v>
       </c>
       <c r="AZ6">
         <f t="shared" si="35"/>
-        <v>1.4267761930706339E-4</v>
+        <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
+      <c r="A8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="B9" s="3">
+      <c r="A9" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9" s="18">
         <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>15</v>
+      <c r="A10" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
+    <row r="11" spans="1:52" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" s="21">
         <v>18.2</v>
       </c>
     </row>
@@ -7455,7 +7559,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -7464,19 +7568,19 @@
     </row>
     <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -8031,642 +8135,642 @@
   <sheetData>
     <row r="1" spans="1:211" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AB1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AC1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AD1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AE1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AF1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AG1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AH1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AL1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AM1" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AN1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AO1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AP1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AR1" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AS1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AT1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="AU1" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="AT1" s="9" t="s">
+      <c r="AV1" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AU1" s="9" t="s">
+      <c r="AW1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AV1" s="9" t="s">
+      <c r="AX1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="AW1" s="9" t="s">
+      <c r="AY1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="AX1" s="9" t="s">
+      <c r="AZ1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="AY1" s="9" t="s">
+      <c r="BA1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="BB1" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BC1" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="BB1" s="9" t="s">
+      <c r="BD1" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="BC1" s="9" t="s">
+      <c r="BE1" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="BD1" s="9" t="s">
+      <c r="BF1" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="BE1" s="9" t="s">
+      <c r="BG1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="BF1" s="9" t="s">
+      <c r="BH1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="BG1" s="9" t="s">
+      <c r="BI1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="BH1" s="9" t="s">
+      <c r="BJ1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="BI1" s="9" t="s">
+      <c r="BK1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="BJ1" s="9" t="s">
+      <c r="BL1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="BK1" s="9" t="s">
+      <c r="BM1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="BL1" s="9" t="s">
+      <c r="BN1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="BM1" s="9" t="s">
+      <c r="BO1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="BN1" s="9" t="s">
+      <c r="BP1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="BO1" s="9" t="s">
+      <c r="BQ1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="BP1" s="9" t="s">
+      <c r="BR1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="BQ1" s="9" t="s">
+      <c r="BS1" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="BR1" s="9" t="s">
+      <c r="BT1" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="BS1" s="9" t="s">
+      <c r="BU1" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="BT1" s="9" t="s">
+      <c r="BV1" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="BU1" s="9" t="s">
+      <c r="BW1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="BV1" s="9" t="s">
+      <c r="BX1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="BW1" s="9" t="s">
+      <c r="BY1" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="BX1" s="9" t="s">
+      <c r="BZ1" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BY1" s="9" t="s">
+      <c r="CA1" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BZ1" s="9" t="s">
+      <c r="CB1" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="CA1" s="9" t="s">
+      <c r="CC1" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="CB1" s="9" t="s">
+      <c r="CD1" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="CC1" s="9" t="s">
+      <c r="CE1" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="CD1" s="9" t="s">
+      <c r="CF1" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="CE1" s="9" t="s">
+      <c r="CG1" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="CF1" s="9" t="s">
+      <c r="CH1" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="CG1" s="9" t="s">
+      <c r="CI1" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="CH1" s="9" t="s">
+      <c r="CJ1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="CI1" s="9" t="s">
+      <c r="CK1" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="CJ1" s="9" t="s">
+      <c r="CL1" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="CK1" s="9" t="s">
+      <c r="CM1" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="CL1" s="9" t="s">
+      <c r="CN1" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="CM1" s="9" t="s">
+      <c r="CO1" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="CN1" s="9" t="s">
+      <c r="CP1" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="CO1" s="9" t="s">
+      <c r="CQ1" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="CP1" s="9" t="s">
+      <c r="CR1" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="CQ1" s="9" t="s">
+      <c r="CS1" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="CR1" s="9" t="s">
+      <c r="CT1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="CS1" s="9" t="s">
+      <c r="CU1" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="CT1" s="9" t="s">
+      <c r="CV1" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="CU1" s="9" t="s">
+      <c r="CW1" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="CV1" s="9" t="s">
+      <c r="CX1" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="CW1" s="9" t="s">
+      <c r="CY1" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="CX1" s="9" t="s">
+      <c r="CZ1" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="CY1" s="9" t="s">
+      <c r="DA1" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="CZ1" s="9" t="s">
+      <c r="DB1" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="DA1" s="9" t="s">
+      <c r="DC1" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="DB1" s="9" t="s">
+      <c r="DD1" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="DC1" s="9" t="s">
+      <c r="DE1" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="DD1" s="9" t="s">
+      <c r="DF1" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="DE1" s="9" t="s">
+      <c r="DG1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="DF1" s="9" t="s">
+      <c r="DH1" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="DG1" s="9" t="s">
+      <c r="DI1" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="DH1" s="9" t="s">
+      <c r="DJ1" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="DI1" s="9" t="s">
+      <c r="DK1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="DJ1" s="9" t="s">
+      <c r="DL1" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="DK1" s="9" t="s">
+      <c r="DM1" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="DL1" s="9" t="s">
+      <c r="DN1" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="DM1" s="9" t="s">
+      <c r="DO1" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="DN1" s="9" t="s">
+      <c r="DP1" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="DO1" s="9" t="s">
+      <c r="DQ1" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="DP1" s="9" t="s">
+      <c r="DR1" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="DQ1" s="9" t="s">
+      <c r="DS1" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="DR1" s="9" t="s">
+      <c r="DT1" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="DS1" s="9" t="s">
+      <c r="DU1" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="DT1" s="9" t="s">
+      <c r="DV1" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="DU1" s="9" t="s">
+      <c r="DW1" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="DV1" s="9" t="s">
+      <c r="DX1" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="DW1" s="9" t="s">
+      <c r="DY1" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="DX1" s="9" t="s">
+      <c r="DZ1" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="DY1" s="9" t="s">
+      <c r="EA1" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="DZ1" s="9" t="s">
+      <c r="EB1" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="EA1" s="9" t="s">
+      <c r="EC1" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="EB1" s="9" t="s">
+      <c r="ED1" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="EC1" s="9" t="s">
+      <c r="EE1" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="ED1" s="9" t="s">
+      <c r="EF1" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="EE1" s="9" t="s">
+      <c r="EG1" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="EF1" s="9" t="s">
+      <c r="EH1" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="EG1" s="9" t="s">
+      <c r="EI1" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="EH1" s="9" t="s">
+      <c r="EJ1" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="EI1" s="9" t="s">
+      <c r="EK1" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="EJ1" s="9" t="s">
+      <c r="EL1" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="EK1" s="9" t="s">
+      <c r="EM1" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="EL1" s="9" t="s">
+      <c r="EN1" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="EM1" s="9" t="s">
+      <c r="EO1" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="EN1" s="9" t="s">
+      <c r="EP1" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="EO1" s="9" t="s">
+      <c r="EQ1" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="EP1" s="9" t="s">
+      <c r="ER1" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="EQ1" s="9" t="s">
+      <c r="ES1" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="ER1" s="9" t="s">
+      <c r="ET1" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="ES1" s="9" t="s">
+      <c r="EU1" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="ET1" s="9" t="s">
+      <c r="EV1" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="EU1" s="9" t="s">
+      <c r="EW1" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="EV1" s="9" t="s">
+      <c r="EX1" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="EW1" s="9" t="s">
+      <c r="EY1" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="EX1" s="9" t="s">
+      <c r="EZ1" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="EY1" s="9" t="s">
+      <c r="FA1" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="EZ1" s="9" t="s">
+      <c r="FB1" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="FA1" s="9" t="s">
+      <c r="FC1" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="FB1" s="9" t="s">
+      <c r="FD1" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="FC1" s="9" t="s">
+      <c r="FE1" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="FD1" s="9" t="s">
+      <c r="FF1" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="FE1" s="9" t="s">
+      <c r="FG1" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="FF1" s="9" t="s">
+      <c r="FH1" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="FG1" s="9" t="s">
+      <c r="FI1" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="FH1" s="9" t="s">
+      <c r="FJ1" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="FI1" s="9" t="s">
+      <c r="FK1" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="FJ1" s="9" t="s">
+      <c r="FL1" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="FK1" s="9" t="s">
+      <c r="FM1" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="FL1" s="9" t="s">
+      <c r="FN1" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="FM1" s="9" t="s">
+      <c r="FO1" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="FN1" s="9" t="s">
+      <c r="FP1" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="FO1" s="9" t="s">
+      <c r="FQ1" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="FP1" s="9" t="s">
+      <c r="FR1" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="FQ1" s="9" t="s">
+      <c r="FS1" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="FR1" s="9" t="s">
+      <c r="FT1" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="FS1" s="9" t="s">
+      <c r="FU1" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="FT1" s="9" t="s">
+      <c r="FV1" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="FU1" s="9" t="s">
+      <c r="FW1" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="FV1" s="9" t="s">
+      <c r="FX1" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="FW1" s="9" t="s">
+      <c r="FY1" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="FX1" s="9" t="s">
+      <c r="FZ1" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="FY1" s="9" t="s">
+      <c r="GA1" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="FZ1" s="9" t="s">
+      <c r="GB1" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="GA1" s="9" t="s">
+      <c r="GC1" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="GB1" s="9" t="s">
+      <c r="GD1" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="GC1" s="9" t="s">
+      <c r="GE1" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="GD1" s="9" t="s">
+      <c r="GF1" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="GE1" s="9" t="s">
+      <c r="GG1" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="GF1" s="9" t="s">
+      <c r="GH1" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="GG1" s="9" t="s">
+      <c r="GI1" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="GH1" s="9" t="s">
+      <c r="GJ1" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="GI1" s="9" t="s">
+      <c r="GK1" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="GJ1" s="9" t="s">
+      <c r="GL1" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="GK1" s="9" t="s">
+      <c r="GM1" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="GL1" s="9" t="s">
+      <c r="GN1" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="GM1" s="9" t="s">
+      <c r="GO1" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="GN1" s="9" t="s">
+      <c r="GP1" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="GO1" s="9" t="s">
+      <c r="GQ1" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="GP1" s="9" t="s">
+      <c r="GR1" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="GQ1" s="9" t="s">
+      <c r="GS1" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="GR1" s="9" t="s">
+      <c r="GT1" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="GS1" s="9" t="s">
+      <c r="GU1" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="GT1" s="9" t="s">
+      <c r="GV1" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="GU1" s="9" t="s">
+      <c r="GW1" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="GV1" s="9" t="s">
+      <c r="GX1" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="GW1" s="9" t="s">
+      <c r="GY1" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="GX1" s="9" t="s">
+      <c r="GZ1" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="GY1" s="9" t="s">
+      <c r="HA1" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="GZ1" s="9" t="s">
+      <c r="HB1" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="HA1" s="9" t="s">
+      <c r="HC1" s="9" t="s">
         <v>236</v>
-      </c>
-      <c r="HB1" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="HC1" s="9" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:211" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -8910,203 +9014,203 @@
       </c>
       <c r="CD2" cm="1">
         <f t="array" ref="CD2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CE2:$HC2,"&gt;0")+1)</f>
-        <v>1.4267761930706339E-4</v>
+        <v>0</v>
       </c>
       <c r="CE2" cm="1">
         <f t="array" ref="CE2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CF2:$HC2,"&gt;0")+1)</f>
-        <v>1.8955794509232236E-4</v>
+        <v>9.1382034038435014E-6</v>
       </c>
       <c r="CF2" cm="1">
         <f t="array" ref="CF2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CG2:$HC2,"&gt;0")+1)</f>
-        <v>2.5087501887319789E-4</v>
+        <v>2.1278993721771694E-5</v>
       </c>
       <c r="CG2" cm="1">
         <f t="array" ref="CG2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CH2:$HC2,"&gt;0")+1)</f>
-        <v>3.3044034177507329E-4</v>
+        <v>3.7347014498544394E-5</v>
       </c>
       <c r="CH2" cm="1">
         <f t="array" ref="CH2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CI2:$HC2,"&gt;0")+1)</f>
-        <v>4.3286275766671886E-4</v>
+        <v>5.8511027962194154E-5</v>
       </c>
       <c r="CI2" cm="1">
         <f t="array" ref="CI2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CJ2:$HC2,"&gt;0")+1)</f>
-        <v>5.6365138676737212E-4</v>
+        <v>8.6234983160760257E-5</v>
       </c>
       <c r="CJ2" cm="1">
         <f t="array" ref="CJ2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CK2:$HC2,"&gt;0")+1)</f>
-        <v>7.2931278684615916E-4</v>
+        <v>1.223356767814851E-4</v>
       </c>
       <c r="CK2" cm="1">
         <f t="array" ref="CK2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CL2:$HC2,"&gt;0")+1)</f>
-        <v>9.3743521238418524E-4</v>
+        <v>1.6904663694182346E-4</v>
       </c>
       <c r="CL2" cm="1">
         <f t="array" ref="CL2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CM2:$HC2,"&gt;0")+1)</f>
-        <v>1.1967512543959785E-3</v>
+        <v>2.2908740360373135E-4</v>
       </c>
       <c r="CM2" cm="1">
         <f t="array" ref="CM2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CN2:$HC2,"&gt;0")+1)</f>
-        <v>1.5171686316344021E-3</v>
+        <v>3.0573682093763767E-4</v>
       </c>
       <c r="CN2" cm="1">
         <f t="array" ref="CN2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CO2:$HC2,"&gt;0")+1)</f>
-        <v>1.9097576064443841E-3</v>
+        <v>4.0290830179875493E-4</v>
       </c>
       <c r="CO2" cm="1">
         <f t="array" ref="CO2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CP2:$HC2,"&gt;0")+1)</f>
-        <v>2.3866825805346267E-3</v>
+        <v>5.2522428621511478E-4</v>
       </c>
       <c r="CP2" cm="1">
         <f t="array" ref="CP2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CQ2:$HC2,"&gt;0")+1)</f>
-        <v>2.9610650716444878E-3</v>
+        <v>6.7808631872770661E-4</v>
       </c>
       <c r="CQ2" cm="1">
         <f t="array" ref="CQ2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CR2:$HC2,"&gt;0")+1)</f>
-        <v>3.6467656742491285E-3</v>
+        <v>8.6773634967242809E-4</v>
       </c>
       <c r="CR2" cm="1">
         <f t="array" ref="CR2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CS2:$HC2,"&gt;0")+1)</f>
-        <v>4.4580739526365112E-3</v>
+        <v>1.1013040715007754E-3</v>
       </c>
       <c r="CS2" cm="1">
         <f t="array" ref="CS2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CT2:$HC2,"&gt;0")+1)</f>
-        <v>5.4092976646944249E-3</v>
+        <v>1.3868343934000575E-3</v>
       </c>
       <c r="CT2" cm="1">
         <f t="array" ref="CT2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CU2:$HC2,"&gt;0")+1)</f>
-        <v>6.5142463855848223E-3</v>
+        <v>1.7332886065554501E-3</v>
       </c>
       <c r="CU2" cm="1">
         <f t="array" ref="CU2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CV2:$HC2,"&gt;0")+1)</f>
-        <v>7.7856095396596492E-3</v>
+        <v>2.1505124765873172E-3</v>
       </c>
       <c r="CV2" cm="1">
         <f t="array" ref="CV2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CW2:$HC2,"&gt;0")+1)</f>
-        <v>9.2342350138447729E-3</v>
+        <v>2.6491645002322903E-3</v>
       </c>
       <c r="CW2" cm="1">
         <f t="array" ref="CW2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CX2:$HC2,"&gt;0")+1)</f>
-        <v>1.0868321764506451E-2</v>
+        <v>3.2405979587188634E-3</v>
       </c>
       <c r="CX2" cm="1">
         <f t="array" ref="CX2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CY2:$HC2,"&gt;0")+1)</f>
-        <v>1.2692547868771803E-2</v>
+        <v>3.9366912592997665E-3</v>
       </c>
       <c r="CY2" cm="1">
         <f t="array" ref="CY2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(CZ2:$HC2,"&gt;0")+1)</f>
-        <v>1.4707163909978713E-2</v>
+        <v>4.7496224302932752E-3</v>
       </c>
       <c r="CZ2" cm="1">
         <f t="array" ref="CZ2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DA2:$HC2,"&gt;0")+1)</f>
-        <v>1.6907089904774603E-2</v>
+        <v>5.6915855493568854E-3</v>
       </c>
       <c r="DA2" cm="1">
         <f t="array" ref="DA2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DB2:$HC2,"&gt;0")+1)</f>
-        <v>1.9281061554515685E-2</v>
+        <v>6.7744493318285534E-3</v>
       </c>
       <c r="DB2" cm="1">
         <f t="array" ref="DB2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DC2:$HC2,"&gt;0")+1)</f>
-        <v>2.1810877745534557E-2</v>
+        <v>8.0093610382538979E-3</v>
       </c>
       <c r="DC2" cm="1">
         <f t="array" ref="DC2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DD2:$HC2,"&gt;0")+1)</f>
-        <v>2.4470805217893771E-2</v>
+        <v>9.4063021858778219E-3</v>
       </c>
       <c r="DD2" cm="1">
         <f t="array" ref="DD2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DE2:$HC2,"&gt;0")+1)</f>
-        <v>2.7227197490210825E-2</v>
+        <v>1.0973606130413696E-2</v>
       </c>
       <c r="DE2" cm="1">
         <f t="array" ref="DE2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DF2:$HC2,"&gt;0")+1)</f>
-        <v>3.0038382886396264E-2</v>
+        <v>1.2717451240743808E-2</v>
       </c>
       <c r="DF2" cm="1">
         <f t="array" ref="DF2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DG2:$HC2,"&gt;0")+1)</f>
-        <v>3.2854870440236994E-2</v>
+        <v>1.464134690196635E-2</v>
       </c>
       <c r="DG2" cm="1">
         <f t="array" ref="DG2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DH2:$HC2,"&gt;0")+1)</f>
-        <v>3.5619912364544648E-2</v>
+        <v>1.6745632706200733E-2</v>
       </c>
       <c r="DH2" cm="1">
         <f t="array" ref="DH2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DI2:$HC2,"&gt;0")+1)</f>
-        <v>3.827044775206212E-2</v>
+        <v>1.9027013668366639E-2</v>
       </c>
       <c r="DI2" cm="1">
         <f t="array" ref="DI2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DJ2:$HC2,"&gt;0")+1)</f>
-        <v>4.0738434630281872E-2</v>
+        <v>2.1478155884034345E-2</v>
       </c>
       <c r="DJ2" cm="1">
         <f t="array" ref="DJ2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DK2:$HC2,"&gt;0")+1)</f>
-        <v>4.2952557155367943E-2</v>
+        <v>2.4087367502602947E-2</v>
       </c>
       <c r="DK2" cm="1">
         <f t="array" ref="DK2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DL2:$HC2,"&gt;0")+1)</f>
-        <v>4.4840272649322499E-2</v>
+        <v>2.6838389042682251E-2</v>
       </c>
       <c r="DL2" cm="1">
         <f t="array" ref="DL2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DM2:$HC2,"&gt;0")+1)</f>
-        <v>4.6330140678369047E-2</v>
+        <v>2.9710314815928063E-2</v>
       </c>
       <c r="DM2" cm="1">
         <f t="array" ref="DM2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DN2:$HC2,"&gt;0")+1)</f>
-        <v>4.7354354957917399E-2</v>
+        <v>3.2677663523481532E-2</v>
       </c>
       <c r="DN2" cm="1">
         <f t="array" ref="DN2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DO2:$HC2,"&gt;0")+1)</f>
-        <v>4.7851380175605751E-2</v>
+        <v>3.5710611015631277E-2</v>
       </c>
       <c r="DO2" cm="1">
         <f t="array" ref="DO2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DP2:$HC2,"&gt;0")+1)</f>
-        <v>4.7768581473379368E-2</v>
+        <v>3.8775391934481963E-2</v>
       </c>
       <c r="DP2" cm="1">
         <f t="array" ref="DP2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DQ2:$HC2,"&gt;0")+1)</f>
-        <v>4.7064725842333344E-2</v>
+        <v>4.1834869769455905E-2</v>
       </c>
       <c r="DQ2" cm="1">
         <f t="array" ref="DQ2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DR2:$HC2,"&gt;0")+1)</f>
-        <v>4.571223339725683E-2</v>
+        <v>4.4849267121907947E-2</v>
       </c>
       <c r="DR2" cm="1">
         <f t="array" ref="DR2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DS2:$HC2,"&gt;0")+1)</f>
-        <v>4.3699063554975437E-2</v>
+        <v>4.7777040159170989E-2</v>
       </c>
       <c r="DS2" cm="1">
         <f t="array" ref="DS2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DT2:$HC2,"&gt;0")+1)</f>
-        <v>4.1030137629935015E-2</v>
+        <v>5.0575873874383399E-2</v>
       </c>
       <c r="DT2" cm="1">
         <f t="array" ref="DT2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DU2:$HC2,"&gt;0")+1)</f>
-        <v>3.7728226791890251E-2</v>
+        <v>5.3203768460591126E-2</v>
       </c>
       <c r="DU2" cm="1">
         <f t="array" ref="DU2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DV2:$HC2,"&gt;0")+1)</f>
-        <v>3.3834275964629623E-2</v>
+        <v>5.5620182556684494E-2</v>
       </c>
       <c r="DV2" cm="1">
         <f t="array" ref="DV2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DW2:$HC2,"&gt;0")+1)</f>
-        <v>2.9407198843811155E-2</v>
+        <v>5.7787197238371522E-2</v>
       </c>
       <c r="DW2" cm="1">
         <f t="array" ref="DW2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DX2:$HC2,"&gt;0")+1)</f>
-        <v>2.4523292727533286E-2</v>
+        <v>5.9670666880471963E-2</v>
       </c>
       <c r="DX2" cm="1">
         <f t="array" ref="DX2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DY2:$HC2,"&gt;0")+1)</f>
-        <v>1.9275669922149241E-2</v>
+        <v>6.1241332540332052E-2</v>
       </c>
       <c r="DY2" cm="1">
         <f t="array" ref="DY2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(DZ2:$HC2,"&gt;0")+1)</f>
-        <v>1.3774823353250532E-2</v>
+        <v>6.2475898923969687E-2</v>
       </c>
       <c r="DZ2" cm="1">
         <f t="array" ref="DZ2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(EA2:$HC2,"&gt;0")+1)</f>
-        <v>8.1544757227045572E-3</v>
+        <v>6.3358147578421301E-2</v>
       </c>
       <c r="EA2" cm="1">
         <f t="array" ref="EA2">INDEX(Calculations!$C$6:$AZ$6,COUNTIF(EB2:$HC2,"&gt;0")+1)</f>
-        <v>2.6150091858251345E-3</v>
+        <v>6.3880424710375722E-2</v>
       </c>
       <c r="EB2">
         <v>0</v>

</xml_diff>